<commit_message>
GDE-8149: fix for 3 test cases, GDE-8302 verify changes in local sandbox env
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ03_BaselineSBLC.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ03_BaselineSBLC.xlsx
@@ -1431,47 +1431,47 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>S324072020165643</t>
+          <t>S306102020130023</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="O2" s="46" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="AQ2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="AR2" s="46" t="inlineStr">
@@ -1804,12 +1804,12 @@
       <c r="CO2" s="46" t="n"/>
       <c r="CP2" s="46" t="inlineStr">
         <is>
-          <t>01-Jun-2021</t>
+          <t>19-Jan-2022</t>
         </is>
       </c>
       <c r="CQ2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="CR2" s="46" t="n"/>
@@ -1855,12 +1855,12 @@
       </c>
       <c r="DA2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="DB2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="DC2" s="48" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="DN2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="DO2" s="11" t="inlineStr">
@@ -1931,7 +1931,7 @@
       <c r="DP2" s="11" t="n"/>
       <c r="DQ2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="DR2" s="48" t="inlineStr">
@@ -2401,7 +2401,7 @@
         </is>
       </c>
       <c r="P2" s="1" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="41" t="inlineStr">
         <is>
@@ -2862,12 +2862,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="L2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="M2" s="10" t="inlineStr">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="E2" s="47" t="inlineStr">
@@ -3827,12 +3827,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -3842,7 +3842,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>60000044</t>
+          <t>60001085</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -6653,12 +6653,12 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>60000044</t>
+          <t>60001085</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -7147,7 +7147,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="D2" s="47" t="inlineStr">
@@ -7157,7 +7157,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -7180,7 +7180,7 @@
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>01-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="L2" s="47" t="inlineStr">
@@ -7220,7 +7220,7 @@
       </c>
       <c r="S2" s="46" t="inlineStr">
         <is>
-          <t>01-Jun-2021</t>
+          <t>19-Jan-2022</t>
         </is>
       </c>
       <c r="T2" s="1" t="inlineStr">
@@ -7250,7 +7250,7 @@
       </c>
       <c r="Y2" s="11" t="inlineStr">
         <is>
-          <t>60000044</t>
+          <t>60001085</t>
         </is>
       </c>
       <c r="Z2" s="1" t="inlineStr">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="AI2" s="11" t="inlineStr">
         <is>
-          <t>60000044</t>
+          <t>60001085</t>
         </is>
       </c>
       <c r="AJ2" s="1" t="n"/>
@@ -7634,17 +7634,17 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>BNS3_24072020165643</t>
+          <t>BNS3_06102020130023</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FACBG24072020171254</t>
+          <t>FACBG05102020122445</t>
         </is>
       </c>
       <c r="E2" s="11" t="inlineStr">
         <is>
-          <t>60000044</t>
+          <t>60001085</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -7658,11 +7658,11 @@
         </is>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>02-Jun-2020</t>
+          <t>20-Jan-2021</t>
         </is>
       </c>
       <c r="J2" s="40" t="inlineStr">

</xml_diff>

<commit_message>
GDE-8149 reset the value of loan amount
</commit_message>
<xml_diff>
--- a/DataSet/LoanIQ_DataSet/EVG_PTYLIQ03_BaselineSBLC.xlsx
+++ b/DataSet/LoanIQ_DataSet/EVG_PTYLIQ03_BaselineSBLC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\LoanIQ_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBE8703-1E5B-4CB2-951C-C4A25CC911E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56879C-C023-4785-9B96-AC1BE4AC96F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6879,8 +6879,8 @@
   </sheetPr>
   <dimension ref="A1:EX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7174,7 +7174,7 @@
         <v>247</v>
       </c>
       <c r="J2" s="33">
-        <v>99000</v>
+        <v>100000</v>
       </c>
       <c r="K2" s="33">
         <v>1000</v>

</xml_diff>